<commit_message>
Add code for Ridge
</commit_message>
<xml_diff>
--- a/kanzaki/機械学習パターン_kanzaki.xlsx
+++ b/kanzaki/機械学習パターン_kanzaki.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hajime\Documents\TopSE\実践演習\github\team\kanzaki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3942757C-208D-4BA1-ABF4-578A37236CC7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A83C84-3314-45B2-AD9A-EFDB6242AEC5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12080" xr2:uid="{36E6B7FA-6078-479A-8CF7-CA0046404250}"/>
   </bookViews>
@@ -696,6 +696,7 @@
   </si>
   <si>
     <t>次元数が多いとクラスタ分類が適切に行われない可能性が高いため、事前にPCA等で次元削減することが望ましい
+分類対象のパラメータは標準化する
 削減する次元数は、Explained varianceの累積値がが90~99%程度になる程度の特長数とするのが一般的
 適切なクラスタ数は、Elbow法、Silhouette法で収束するところを探索</t>
     <rPh sb="0" eb="2">
@@ -738,51 +739,60 @@
       <t>ノゾ</t>
     </rPh>
     <rPh sb="53" eb="55">
+      <t>ブンルイ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="64" eb="67">
+      <t>ヒョウジュンカ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
       <t>サクゲン</t>
     </rPh>
-    <rPh sb="57" eb="59">
+    <rPh sb="74" eb="76">
       <t>ジゲン</t>
     </rPh>
-    <rPh sb="59" eb="60">
+    <rPh sb="76" eb="77">
       <t>スウ</t>
     </rPh>
-    <rPh sb="81" eb="83">
+    <rPh sb="98" eb="100">
       <t>ルイセキ</t>
     </rPh>
-    <rPh sb="83" eb="84">
+    <rPh sb="100" eb="101">
       <t>チ</t>
     </rPh>
-    <rPh sb="92" eb="94">
+    <rPh sb="109" eb="111">
       <t>テイド</t>
     </rPh>
-    <rPh sb="97" eb="99">
+    <rPh sb="114" eb="116">
       <t>テイド</t>
     </rPh>
-    <rPh sb="100" eb="102">
+    <rPh sb="117" eb="119">
       <t>トクチョウ</t>
-    </rPh>
-    <rPh sb="102" eb="103">
-      <t>スウ</t>
-    </rPh>
-    <rPh sb="108" eb="111">
-      <t>イッパンテキ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>テキセツ</t>
     </rPh>
     <rPh sb="119" eb="120">
       <t>スウ</t>
     </rPh>
-    <rPh sb="127" eb="128">
+    <rPh sb="125" eb="128">
+      <t>イッパンテキ</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>テキセツ</t>
+    </rPh>
+    <rPh sb="136" eb="137">
+      <t>スウ</t>
+    </rPh>
+    <rPh sb="144" eb="145">
       <t>ホウ</t>
     </rPh>
-    <rPh sb="139" eb="140">
+    <rPh sb="156" eb="157">
       <t>ホウ</t>
     </rPh>
-    <rPh sb="141" eb="143">
+    <rPh sb="158" eb="160">
       <t>シュウソク</t>
     </rPh>
-    <rPh sb="149" eb="151">
+    <rPh sb="166" eb="168">
       <t>タンサク</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -1173,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DC1A42-B505-4165-9AA1-B9DE7A1F4799}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>